<commit_message>
write the code common methods and excel reader. write the input json and register json and create logger report file.
</commit_message>
<xml_diff>
--- a/API_Assignment/Resources/test_data.xlsx
+++ b/API_Assignment/Resources/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rkunchala/pythonAssignments/Python_Assignments/API_Assignment/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE8DCB3-FF24-4D44-A807-670E876EB820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746512FF-5F0F-C849-AF25-EEB69519951F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,41 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>Credit card</t>
-  </si>
-  <si>
-    <t>Raju</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Ongole</t>
-  </si>
-  <si>
-    <t>Nithish</t>
-  </si>
-  <si>
-    <t>Tamilnadu</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -434,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -450,64 +416,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="3">
-        <v>123456789012345</v>
-      </c>
-      <c r="E2">
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <v>2025</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3">
-        <v>123456789012945</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="F3">
-        <v>2025</v>
-      </c>
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -518,7 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B6A37B-6AC7-9943-A902-95773952D757}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>

</xml_diff>